<commit_message>
fix: Corrección de archivos para mejorar procesos
</commit_message>
<xml_diff>
--- a/media/Consolidado PMIRS Julio 2025.xlsx
+++ b/media/Consolidado PMIRS Julio 2025.xlsx
@@ -64,7 +64,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,11 +440,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="31" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="36" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,36 +467,52 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Peso / Cantidad</t>
+          <t>Peso</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Costo Total</t>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Costo_Unitario</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Costo_Total</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Aprovechable</t>
+          <t>Respel Aprovechable</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Papel Archivo - KG</t>
+          <t>Batería Ácido Plomo 30-31H - UND</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>26-07-25</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>40000</v>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1127.46</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>2483</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>2799483</v>
       </c>
     </row>
     <row r="3">
@@ -505,65 +523,170 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Papel Periódico - KG</t>
+          <t>Radiador Cobre - KG</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>26-07-25</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>30000</v>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>124.2</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>7200</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>894240</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Aprovechable</t>
+          <t>Respel Aprovechable</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Plástico por Seleccionar - KG</t>
+          <t>Aceite Usado - KG</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>26-07-25</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>42300</v>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2976.38</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>352</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>1047686</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>Respel</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Refrigerante - KG</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>1210</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1428</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1727880</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Especial</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Fibra de Vidrio - MT3</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>84300</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>337200</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Respel Aprovechable</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Batería Ácido Plomo 65-G4-27 - UND</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>2066</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
           <t>Aprovechable</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Aluminio Sucio - KG</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>01-07-25</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>97500</v>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Papel Archivo - KG</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>07-07-25</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>400</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>40000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>